<commit_message>
updated tables with new data (nestedness)
</commit_message>
<xml_diff>
--- a/Tables_Figures/Table_SimulateDistributions.xlsx
+++ b/Tables_Figures/Table_SimulateDistributions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="31">
   <si>
     <t>Covariate Effect Values</t>
   </si>
@@ -83,9 +83,6 @@
     </r>
   </si>
   <si>
-    <t>*** Bold means this structure was more likely in the simulations</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -142,6 +139,98 @@
   </si>
   <si>
     <t>Clementsian/Gleasonian</t>
+  </si>
+  <si>
+    <t>Random/Nested/Quasi-Nested/Quasi-Clementsian</t>
+  </si>
+  <si>
+    <t>Random/Quasi-Nested/Nested</t>
+  </si>
+  <si>
+    <t>Quasi-Nested/Nested</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quasi-Nested</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Nested</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nested</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Quasi-Nested/Quasi-Clementsian</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quasi-Nested</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Random</t>
+    </r>
+  </si>
+  <si>
+    <t>Bold means this structure was more likely in the simulations</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Table 2. Nested patterns</t>
+  </si>
+  <si>
+    <t>Table 1. Gleasonian and Clementsian patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The point of Table 2 is that nested patterns can arise due to the range of covariate values. </t>
   </si>
 </sst>
 </file>
@@ -205,7 +294,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -273,21 +362,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -321,6 +431,15 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -354,6 +473,15 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -697,82 +825,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>0.6</v>
-      </c>
-      <c r="B3">
-        <v>0.7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
@@ -787,6 +894,9 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
@@ -794,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -813,14 +923,17 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
@@ -839,14 +952,17 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -860,22 +976,22 @@
         <v>0.7</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>0.5</v>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" t="s">
         <v>8</v>
@@ -904,13 +1020,10 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -930,16 +1043,19 @@
         <v>0.5</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I9" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -962,13 +1078,13 @@
         <v>7</v>
       </c>
       <c r="G10">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -985,19 +1101,19 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1023,10 +1139,10 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1046,16 +1162,16 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1078,13 +1194,13 @@
         <v>7</v>
       </c>
       <c r="G14">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="I14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1095,25 +1211,25 @@
         <v>0.7</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1139,13 +1255,13 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>0.6</v>
       </c>
@@ -1162,19 +1278,19 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G17">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>0.6</v>
       </c>
@@ -1194,45 +1310,45 @@
         <v>7</v>
       </c>
       <c r="G18">
+        <v>-1</v>
+      </c>
+      <c r="H18">
+        <v>-1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>0.6</v>
+      </c>
+      <c r="B19">
+        <v>0.7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19">
         <v>-4</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>4</v>
       </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19">
-        <v>0.6</v>
-      </c>
-      <c r="B19">
-        <v>0.7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>-3</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
       <c r="I19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>0.6</v>
       </c>
@@ -1255,13 +1371,13 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>0.6</v>
       </c>
@@ -1278,19 +1394,19 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G21">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>0.6</v>
       </c>
@@ -1310,20 +1426,345 @@
         <v>7</v>
       </c>
       <c r="G22">
+        <v>-1</v>
+      </c>
+      <c r="H22">
+        <v>-1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>0.6</v>
+      </c>
+      <c r="B23">
+        <v>0.7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>-3</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23">
         <v>-4</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>4</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>0.6</v>
+      </c>
+      <c r="B29">
+        <v>0.7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>0.6</v>
+      </c>
+      <c r="B30">
+        <v>0.7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>-1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>0.6</v>
+      </c>
+      <c r="B31">
+        <v>0.7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>-1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>0.6</v>
+      </c>
+      <c r="B32">
+        <v>0.7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>10</v>
+      </c>
+      <c r="I32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>0.6</v>
+      </c>
+      <c r="B33">
+        <v>0.7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>-3</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>0.6</v>
+      </c>
+      <c r="B34">
+        <v>0.7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>-3</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>0.6</v>
+      </c>
+      <c r="B35">
+        <v>0.7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>-3</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>0.6</v>
+      </c>
+      <c r="B36">
+        <v>0.7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>-3</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:I2"/>
+  <mergeCells count="7">
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="I27:I28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>